<commit_message>
Added production losses display
</commit_message>
<xml_diff>
--- a/Code/Overlap/Sol Check 2.xlsx
+++ b/Code/Overlap/Sol Check 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA0971-C95D-4309-8393-A28B7085CBC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B99445C-5E6E-4F2C-9A9D-FF9FC8504867}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B301433D-9DCC-4BFC-86CA-DD685E12B0B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B301433D-9DCC-4BFC-86CA-DD685E12B0B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessels" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>Vessels</t>
   </si>
@@ -197,6 +197,48 @@
   </si>
   <si>
     <t>Up %</t>
+  </si>
+  <si>
+    <t>Energy Avail</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Prod losses</t>
+  </si>
+  <si>
+    <t>"Total" energy</t>
+  </si>
+  <si>
+    <t>Strath</t>
+  </si>
+  <si>
+    <t>NOWI</t>
+  </si>
+  <si>
+    <t>UiS Sim</t>
+  </si>
+  <si>
+    <t>ECUME</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Time Avail</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Total Costs 1</t>
+  </si>
+  <si>
+    <t>Total Costs 2</t>
+  </si>
+  <si>
+    <t>My (720 days, 720 max work, 142 ppMWh)</t>
   </si>
 </sst>
 </file>
@@ -23016,8 +23058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6454C125-6E03-4F36-99C8-C5F99DD47F1F}">
   <dimension ref="A1:AM619"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AC34" sqref="AC34:AC39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25896,7 +25938,7 @@
         <v>0.40656249999999999</v>
       </c>
       <c r="AB34" s="3">
-        <f t="shared" ref="AB34:AB40" si="17">SUM(W34:AA34)</f>
+        <f t="shared" ref="AB34:AB39" si="17">SUM(W34:AA34)</f>
         <v>0.71872395833333336</v>
       </c>
       <c r="AC34" s="3">
@@ -61396,18 +61438,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9D08A3-6FCF-4074-9B9B-D626A1B91044}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>41</v>
       </c>
@@ -61417,8 +61460,29 @@
       <c r="F1">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -61426,8 +61490,30 @@
         <f>Failures!AC39</f>
         <v>24.328124999999989</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2">
+        <v>83.7</v>
+      </c>
+      <c r="N2">
+        <v>83.74</v>
+      </c>
+      <c r="O2">
+        <v>84.4</v>
+      </c>
+      <c r="P2">
+        <v>80.819999999999993</v>
+      </c>
+      <c r="Q2">
+        <v>83.16</v>
+      </c>
+      <c r="R2">
+        <f>R3</f>
+        <v>93.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -61435,8 +61521,29 @@
         <f>B2</f>
         <v>24.328124999999989</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3">
+        <v>82.11</v>
+      </c>
+      <c r="N3">
+        <v>82.86</v>
+      </c>
+      <c r="O3">
+        <v>84</v>
+      </c>
+      <c r="P3">
+        <v>81.7</v>
+      </c>
+      <c r="Q3">
+        <v>82.67</v>
+      </c>
+      <c r="R3">
+        <v>93.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -61448,8 +61555,29 @@
         <f>B4/1000000</f>
         <v>7.2016140000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4">
+        <v>17.28</v>
+      </c>
+      <c r="N4">
+        <v>16.63</v>
+      </c>
+      <c r="O4">
+        <v>15.48</v>
+      </c>
+      <c r="P4">
+        <v>18.64</v>
+      </c>
+      <c r="Q4">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="R4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -61461,8 +61589,47 @@
         <f t="shared" ref="C5:C8" si="0">B5/1000000</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5">
+        <f>100*M4/(100-M3)</f>
+        <v>96.590273896031306</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:U5" si="1">100*N4/(100-N3)</f>
+        <v>97.024504084013998</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>96.75</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>101.85792349726778</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>98.153491055972324</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>98.187311178247668</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -61474,8 +61641,29 @@
         <f t="shared" si="0"/>
         <v>5.6902499999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>17.84</v>
+      </c>
+      <c r="N6">
+        <v>19.18</v>
+      </c>
+      <c r="O6">
+        <v>12.24</v>
+      </c>
+      <c r="P6">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Q6">
+        <v>14.64</v>
+      </c>
+      <c r="R6">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -61486,8 +61674,30 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7">
+        <v>22.44</v>
+      </c>
+      <c r="N7">
+        <v>25.17</v>
+      </c>
+      <c r="O7">
+        <v>17.93</v>
+      </c>
+      <c r="P7">
+        <v>14.48</v>
+      </c>
+      <c r="Q7">
+        <v>20</v>
+      </c>
+      <c r="R7">
+        <f>R6</f>
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -61497,6 +61707,70 @@
       <c r="C8" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
+      </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8">
+        <f>M4+M6</f>
+        <v>35.120000000000005</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:S8" si="2">N4+N6</f>
+        <v>35.81</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>27.72</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>27.94</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>31.650000000000002</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>12.18</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9">
+        <f>M4+M7</f>
+        <v>39.72</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:S9" si="3">N4+N7</f>
+        <v>41.8</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>33.409999999999997</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>33.120000000000005</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>37.010000000000005</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>12.18</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>